<commit_message>
Code and readme update
</commit_message>
<xml_diff>
--- a/Parts_and_costs.xlsx
+++ b/Parts_and_costs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuba\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuba\Documents\Arduino\RatElevator\RatElevator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -762,7 +762,7 @@
   <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>